<commit_message>
rearranged inf GUI, cleaned up readme and confirmed units on eelc and eion in reader
</commit_message>
<xml_diff>
--- a/data/experimental/FeSi_s77742.xlsx
+++ b/data/experimental/FeSi_s77742.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cjkri\PycharmProjects\pyhy\data\experimental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62332205-FEB9-44DE-A51A-CD019948EE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F1FB3F-C446-457C-B07B-A3C6E0B11E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{7F63B9CF-C652-4E17-9441-712E762B7D2A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" activeTab="1" xr2:uid="{7F63B9CF-C652-4E17-9441-712E762B7D2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Shot Number</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>VISAR U (km/s)</t>
+  </si>
+  <si>
+    <t>https://www.osti.gov/pages/biblio/1634289</t>
   </si>
 </sst>
 </file>
@@ -506,7 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7A68F4-3CC3-4BD2-BFE5-BBE77249D11E}">
   <dimension ref="A1:F1102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -16339,10 +16342,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E79E3363-1F8D-48A1-B959-DFF407837AB4}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16470,6 +16473,11 @@
         <v>23</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>